<commit_message>
Refacto + correction code
</commit_message>
<xml_diff>
--- a/Jeux de donnees/SFCC/Connection/jdd-Connection.xlsx
+++ b/Jeux de donnees/SFCC/Connection/jdd-Connection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_aggour_groupeonepoint_com/Documents/Clarins/clarins-auto-uat-ihm/Jeux de donnees/SFCC/Connection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onepoint365-my.sharepoint.com/personal/s_ramos-izquierdo_groupeonepoint_com/Documents/Bureau/Clarins/Outils/clarins_auto_uat_ihm/Jeux de donnees/SFCC/Connection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4125495-AB95-AA4D-9C69-02F3CAFE833C}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{F2498E7F-A211-5648-BD84-328060702354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83AD3CA5-FDD5-4C2F-91E3-558253AC6C8F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DDB3DD0-E88E-8949-89B8-E2C45E0A4C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -68,9 +68,6 @@
     <t>ITA</t>
   </si>
   <si>
-    <t>UK</t>
-  </si>
-  <si>
     <t>CHE</t>
   </si>
   <si>
@@ -116,14 +113,38 @@
     <t>***Description***</t>
   </si>
   <si>
-    <t>This email adress has 3 Ids in step (3 accounts)</t>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>${regions}</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>LUX</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>UC7_SFCC_Connect_UAT</t>
+  </si>
+  <si>
+    <t>UC8_SFCC_Connect_UAT</t>
+  </si>
+  <si>
+    <t>URL HS</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -654,23 +675,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BC4A3E-ED2A-A240-8C79-297922065A66}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="30.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="23.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -680,19 +703,22 @@
       <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>25</v>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="10" customFormat="1" ht="21">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -700,19 +726,18 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="21">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -720,16 +745,18 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="10" customFormat="1" ht="21">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -737,66 +764,120 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="10" customFormat="1" ht="21">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" s="10" customFormat="1" ht="21">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="G6" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="21">
+      <c r="A7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="22" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="21">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" s="10" customFormat="1" ht="21">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B7">
+  <conditionalFormatting sqref="B2:B9">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -804,7 +885,7 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
+  <conditionalFormatting sqref="C2:D2">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -812,7 +893,7 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D3">
+  <conditionalFormatting sqref="E1 E3">
     <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"YES"</formula>
     </cfRule>

</xml_diff>